<commit_message>
fixed passenger and class
</commit_message>
<xml_diff>
--- a/test-data/flightData.xlsx
+++ b/test-data/flightData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tung/Documents/Project/agoda-flight-automation/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63313EA8-0258-A248-82D6-73E497DA753D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8313D0-1822-E042-8897-75323773D12E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16180" xr2:uid="{E1C80E68-E4FE-A948-8981-AFB864D45E95}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>futureDay</t>
   </si>
@@ -59,6 +59,15 @@
   </si>
   <si>
     <t>Barcelona</t>
+  </si>
+  <si>
+    <t>passenger</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>Economy</t>
   </si>
 </sst>
 </file>
@@ -411,15 +420,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9E6978-1670-2E4F-87F5-3B87BCA6A6E8}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,8 +438,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -440,8 +455,14 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -450,6 +471,12 @@
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>